<commit_message>
carga masiva & cdn
</commit_message>
<xml_diff>
--- a/ecommerce-hs/msvc-admin/src/main/resources/static/plantilla/Plantilla-Productos.xlsx
+++ b/ecommerce-hs/msvc-admin/src/main/resources/static/plantilla/Plantilla-Productos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAWII\ecommerce-microservicios\ecommerce-hs\msvc-admin\src\main\resources\static\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D38F091-1B17-4E16-BCD4-884CFC68063C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1304507-A0C4-41C5-A647-3721B2D779A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C493A801-EAB4-4507-B5C3-F0C694CAB0A8}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{C493A801-EAB4-4507-B5C3-F0C694CAB0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Descripción</t>
-  </si>
-  <si>
     <t>Precio</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>Estado</t>
+  </si>
+  <si>
+    <t>Nombre</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,22 +492,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>